<commit_message>
Update unit test e main per velocizzare gli esperimenti
</commit_message>
<xml_diff>
--- a/risultati_esperimenti_progetto.xlsx
+++ b/risultati_esperimenti_progetto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conca\Documents\progetti\GNO_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC065BFE-26EF-4FD0-8551-85336AD49A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDB7835-0B6F-4E62-8EEB-3344B1F6944C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{10C59D22-31E7-4F4C-95DC-A36B48568401}"/>
   </bookViews>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40A25CA7-3B22-4990-A2EF-43E73A3B564A}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1878,6 +1878,12 @@
       <c r="H44">
         <v>2.5652465519151499E-2</v>
       </c>
+      <c r="I44" s="2">
+        <v>3.8729328155517502</v>
+      </c>
+      <c r="J44">
+        <v>1.05591082663456</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
@@ -1898,6 +1904,18 @@
       <c r="F45">
         <v>5</v>
       </c>
+      <c r="G45">
+        <v>0.654283475875854</v>
+      </c>
+      <c r="H45">
+        <v>6.0748244857041098E-2</v>
+      </c>
+      <c r="I45">
+        <v>2.9005457878112701</v>
+      </c>
+      <c r="J45">
+        <v>0.16064807726299399</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
@@ -1918,19 +1936,21 @@
       <c r="F46">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H48">
-        <v>52</v>
+      <c r="G46">
+        <v>912.27280468940705</v>
       </c>
     </row>
     <row r="49" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F49" s="3"/>
     </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="F51" s="3"/>
+    </row>
     <row r="52" spans="6:7" x14ac:dyDescent="0.35">
       <c r="G52" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>